<commit_message>
Ejercicio de inplementacion completo
</commit_message>
<xml_diff>
--- a/src/test/resources/features/DataDriven/DataRegister.xlsx
+++ b/src/test/resources/features/DataDriven/DataRegister.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bdd-serenity\src\test\resources\features\DataDriven\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB9A1C7D-F817-466A-9695-FC33CDAE881B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C68971D-1B19-4E19-83C3-C30EF21C3FE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{D43456C5-FB75-460C-A99D-6369FF4FEDF2}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
   <si>
     <t>User</t>
   </si>
@@ -137,13 +137,16 @@
   </si>
   <si>
     <t>Jahu*127</t>
+  </si>
+  <si>
+    <t>producto</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,6 +180,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF9876AA"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -199,7 +209,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -208,6 +218,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -523,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36C0D5EE-C4C4-47D8-9BB8-9939E5D019C9}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -536,7 +549,7 @@
     <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -567,8 +580,11 @@
       <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="4" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -599,8 +615,11 @@
       <c r="J2">
         <v>13215</v>
       </c>
+      <c r="K2">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -631,8 +650,11 @@
       <c r="J3">
         <v>13215</v>
       </c>
+      <c r="K3">
+        <v>3</v>
+      </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -663,8 +685,11 @@
       <c r="J4">
         <v>13215</v>
       </c>
+      <c r="K4">
+        <v>3</v>
+      </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -695,8 +720,11 @@
       <c r="J5">
         <v>13215</v>
       </c>
+      <c r="K5">
+        <v>3</v>
+      </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -726,6 +754,9 @@
       </c>
       <c r="J6">
         <v>13215</v>
+      </c>
+      <c r="K6">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>